<commit_message>
add mvdelta method,fix some problems
</commit_message>
<xml_diff>
--- a/data/returns_plainBS.xlsx
+++ b/data/returns_plainBS.xlsx
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>58.69457760110614</v>
+        <v>353107.187292833</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -978,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>312.8098613198461</v>
+        <v>1378423.928730365</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -986,7 +986,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>139.2449173193419</v>
+        <v>562548.9143240415</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -994,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>210.3581856621296</v>
+        <v>329923.1690090631</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1002,7 +1002,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>57.11395038146551</v>
+        <v>297844.1454044107</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>85.68322608157794</v>
+        <v>293830.4731693168</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>34.77612472070579</v>
+        <v>120823.8530767055</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>134.9694494701359</v>
+        <v>861651.5420112604</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1.129174122225733</v>
+        <v>11635.04829994273</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>32.18646749107079</v>
+        <v>241709.3641200779</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-1.081124258866238</v>
+        <v>-9247.423686481659</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>30.04879804682425</v>
+        <v>167866.6053724937</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>70.95039155876736</v>
+        <v>377048.9616766949</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2.106834155435324</v>
+        <v>48012.98230680542</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>21.41932742893129</v>
+        <v>528316.5919680188</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>88.84039518964664</v>
+        <v>247086.5709557616</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>5.464314024953549</v>
+        <v>58099.24171038892</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>53.42586911518197</v>
+        <v>51018.60107299283</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>19.98964235815813</v>
+        <v>1074.49260778324</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.6966689696592071</v>
+        <v>3496.184802702154</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>13.59936280374173</v>
+        <v>52515.70188920992</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>68.72985851053421</v>
+        <v>286895.2489533117</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>3.488715321509844</v>
+        <v>72822.94764810776</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>26.25278751447946</v>
+        <v>252707.7585450946</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>13.98612175135002</v>
+        <v>128523.7742424959</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1170,7 +1170,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>1.585103169118302</v>
+        <v>177.3291271332356</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>16.57725331576034</v>
+        <v>7319.574811562483</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>49.56816169658509</v>
+        <v>241463.7560799776</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>31.85337649267517</v>
+        <v>53712.44526855976</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>17.25445092262504</v>
+        <v>154775.5519589498</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1210,7 +1210,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>18.09513903180636</v>
+        <v>66993.56184435321</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1218,7 +1218,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>95.56242827348241</v>
+        <v>356356.3802516162</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>293.252750082764</v>
+        <v>1399335.951553547</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>40.35286520139616</v>
+        <v>197532.2180734938</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>72.11849248589706</v>
+        <v>78924.01762866895</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>11.86381692031657</v>
+        <v>125234.8120884976</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>18.35151222296955</v>
+        <v>55305.37408942254</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1266,7 +1266,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>12.92812464183719</v>
+        <v>41990.66874496177</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>15.57767903003516</v>
+        <v>31469.11976184614</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>4.132983457254929</v>
+        <v>39476.82899961612</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>-2.668528729781177</v>
+        <v>-9535.158940314954</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1298,7 +1298,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.695775613529537</v>
+        <v>4059.157042438178</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>12.50220034014238</v>
+        <v>91581.23593549331</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>68.05470409435507</v>
+        <v>217906.7406787807</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>28.82221206767481</v>
+        <v>99765.69888141434</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>10.39668668493411</v>
+        <v>2934.534665971266</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>12.96610326991875</v>
+        <v>22444.02913975685</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>26.9499272220071</v>
+        <v>5220.327944377907</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>6.446785540410247</v>
+        <v>307.3229108457849</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>23.27544514207171</v>
+        <v>170345.9171456412</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>28.50360348747502</v>
+        <v>235456.9537979132</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>61.29266764331209</v>
+        <v>178370.7088459181</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>48.49423145750352</v>
+        <v>44532.15994452681</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>30.57314943675421</v>
+        <v>18123.18170018367</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>43.50754331188533</v>
+        <v>146338.9372740175</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>62.10165418339071</v>
+        <v>290533.6945405298</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>130.071903805973</v>
+        <v>206561.4747322037</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0.1082707148476677</v>
+        <v>-1946.725184891479</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>72.75704475943613</v>
+        <v>72492.4876245331</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>3.974120359613256</v>
+        <v>21768.32855536722</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>1.99260558613013</v>
+        <v>23847.89727093175</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>0.595189915564545</v>
+        <v>2794.15066398097</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>20.14114318276707</v>
+        <v>50783.45973144678</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>15.67488369562487</v>
+        <v>110821.6688475885</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>7.728634099955795</v>
+        <v>64613.62578703186</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>50.92096595651059</v>
+        <v>60472.88788957534</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>7.456856071943962</v>
+        <v>4501.508728562553</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0.2923890299411218</v>
+        <v>363.8043122737781</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>28.83596005379063</v>
+        <v>129311.3912572124</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>28.52647124664331</v>
+        <v>188395.5085467592</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1530,7 +1530,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>11.25372943748725</v>
+        <v>41611.50158963933</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1538,7 +1538,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>26.56563334022829</v>
+        <v>1148.338558044093</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1546,7 +1546,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>21.42295846803263</v>
+        <v>21787.63441664202</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1554,7 +1554,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>54.75852350948086</v>
+        <v>22970.34682017438</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1562,7 +1562,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>-4.909179556578573</v>
+        <v>-8711.071480416655</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1570,7 +1570,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>-4.138279833772678</v>
+        <v>-3958.354823243768</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1578,7 +1578,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>-3.252075860435645</v>
+        <v>509.3115530712691</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1586,7 +1586,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>32.76399204118453</v>
+        <v>205101.1194719379</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1594,7 +1594,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>15.56189862552742</v>
+        <v>132368.6006215859</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1602,7 +1602,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>89.92548282188622</v>
+        <v>106523.2588003992</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1610,7 +1610,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>30.3859979378045</v>
+        <v>-362.1150139397707</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1618,7 +1618,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>3.791331769916085</v>
+        <v>32054.56956484991</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1626,7 +1626,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>2.360395311510095</v>
+        <v>10849.68624168212</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1634,7 +1634,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>4.619345098789847</v>
+        <v>57912.43568244346</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1642,7 +1642,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>3.187595208581654</v>
+        <v>8498.451116497909</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1650,7 +1650,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>1.819611646177457</v>
+        <v>34572.32337459434</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1658,7 +1658,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>77.19515115258038</v>
+        <v>133611.1234992857</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1666,7 +1666,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>20.28273711428</v>
+        <v>68816.27736764478</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1674,7 +1674,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>0.9831119540872708</v>
+        <v>744.9515459063349</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>1.993398864795149</v>
+        <v>6750.58112194156</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>0.5850953023234592</v>
+        <v>1402.653256418879</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1698,7 +1698,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>12.00824730913234</v>
+        <v>78970.34576139206</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1706,7 +1706,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>12.94434593279004</v>
+        <v>59212.82186114629</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1714,7 +1714,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>14.18360150715109</v>
+        <v>40515.6313431482</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>19.04461856338605</v>
+        <v>24444.96577490838</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1730,7 +1730,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>184.6111354463452</v>
+        <v>294856.8346528659</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1738,7 +1738,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>15.68779009791085</v>
+        <v>9743.478320329743</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1746,7 +1746,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>5.169638458040903</v>
+        <v>-1227.777310329569</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1754,7 +1754,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>1.255943505195817</v>
+        <v>-428.1642915112931</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1762,7 +1762,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>0.3827356325144084</v>
+        <v>1818.037093691774</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1770,7 +1770,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>-0.05712415591830157</v>
+        <v>-509.0635093416887</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1778,7 +1778,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>2.424425975058028</v>
+        <v>18419.30104860843</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1786,7 +1786,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>17.40467400855518</v>
+        <v>18338.38250663877</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1794,7 +1794,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>7.930361027487844</v>
+        <v>2241.390036389487</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1802,7 +1802,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>15.63969598064539</v>
+        <v>2954.022653930781</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1810,7 +1810,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>-0.2613593585931843</v>
+        <v>-1304.374566210175</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1818,7 +1818,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>31.47199158371692</v>
+        <v>43205.31219464821</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1826,7 +1826,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>24.68055495527767</v>
+        <v>53623.58480725802</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1834,7 +1834,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>30.08554798118367</v>
+        <v>15063.33849903644</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1842,7 +1842,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>6.136787360449156</v>
+        <v>5138.69548737143</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1850,7 +1850,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>13.8811574476827</v>
+        <v>-417.3975405371667</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1858,7 +1858,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>7.010362215871346</v>
+        <v>24877.15296241514</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1866,7 +1866,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>6.122296058915021</v>
+        <v>-9707.928119841868</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1874,7 +1874,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>26.74809933078776</v>
+        <v>-34150.2133206007</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1882,7 +1882,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>23.86393100355441</v>
+        <v>28231.20349459045</v>
       </c>
     </row>
   </sheetData>
@@ -1911,7 +1911,7 @@
         <v>116</v>
       </c>
       <c r="B2">
-        <v>-25.97843228890978</v>
+        <v>-112525.3353716712</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1919,7 +1919,7 @@
         <v>117</v>
       </c>
       <c r="B3">
-        <v>-43.82476133269757</v>
+        <v>-220226.6275647185</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1927,7 +1927,7 @@
         <v>118</v>
       </c>
       <c r="B4">
-        <v>-64.67773759188395</v>
+        <v>-87134.88014656462</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1935,7 +1935,7 @@
         <v>119</v>
       </c>
       <c r="B5">
-        <v>16.51143062163874</v>
+        <v>36998.54545057315</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1943,7 +1943,7 @@
         <v>120</v>
       </c>
       <c r="B6">
-        <v>-32.78176534064215</v>
+        <v>-523804.0365732873</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1951,7 +1951,7 @@
         <v>121</v>
       </c>
       <c r="B7">
-        <v>-20.62808710421942</v>
+        <v>-94494.66814890664</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1959,7 +1959,7 @@
         <v>122</v>
       </c>
       <c r="B8">
-        <v>-26.37828038090965</v>
+        <v>-211871.4579099077</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1967,7 +1967,7 @@
         <v>123</v>
       </c>
       <c r="B9">
-        <v>-51.1288812896717</v>
+        <v>-336325.2130963419</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1975,7 +1975,7 @@
         <v>124</v>
       </c>
       <c r="B10">
-        <v>-17.49482861542436</v>
+        <v>-6459.029372520913</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1983,7 +1983,7 @@
         <v>125</v>
       </c>
       <c r="B11">
-        <v>-44.73879688441328</v>
+        <v>-44890.66963154535</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1991,7 +1991,7 @@
         <v>126</v>
       </c>
       <c r="B12">
-        <v>-4.007302928086645</v>
+        <v>-35008.06557954707</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1999,7 +1999,7 @@
         <v>127</v>
       </c>
       <c r="B13">
-        <v>-6.370119205227064</v>
+        <v>-88592.07705054163</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2007,7 +2007,7 @@
         <v>128</v>
       </c>
       <c r="B14">
-        <v>-5.227215081622738</v>
+        <v>-128095.8428729217</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2015,7 +2015,7 @@
         <v>129</v>
       </c>
       <c r="B15">
-        <v>-12.73954232033656</v>
+        <v>-248239.7418018068</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2023,7 +2023,7 @@
         <v>130</v>
       </c>
       <c r="B16">
-        <v>-14.57791605144398</v>
+        <v>-55111.76051292621</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2031,7 +2031,7 @@
         <v>131</v>
       </c>
       <c r="B17">
-        <v>-18.37625551058874</v>
+        <v>-81104.48335492674</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2039,7 +2039,7 @@
         <v>132</v>
       </c>
       <c r="B18">
-        <v>-9.589643227199437</v>
+        <v>-75442.73019933126</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2047,7 +2047,7 @@
         <v>133</v>
       </c>
       <c r="B19">
-        <v>-38.17444793567454</v>
+        <v>-39342.64648530041</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2055,7 +2055,7 @@
         <v>134</v>
       </c>
       <c r="B20">
-        <v>-7.921308393816362</v>
+        <v>-412216.6296682475</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2063,7 +2063,7 @@
         <v>135</v>
       </c>
       <c r="B21">
-        <v>7.743150518359131</v>
+        <v>12066.8826275951</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2071,7 +2071,7 @@
         <v>136</v>
       </c>
       <c r="B22">
-        <v>-4.477452124809488</v>
+        <v>-21588.70325219581</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2079,7 +2079,7 @@
         <v>137</v>
       </c>
       <c r="B23">
-        <v>-13.63243229410629</v>
+        <v>-212861.5303006237</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2087,7 +2087,7 @@
         <v>138</v>
       </c>
       <c r="B24">
-        <v>-46.40420723946445</v>
+        <v>-5378.381620707254</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2095,7 +2095,7 @@
         <v>139</v>
       </c>
       <c r="B25">
-        <v>-17.51550216431544</v>
+        <v>-47125.71596388576</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2103,7 +2103,7 @@
         <v>140</v>
       </c>
       <c r="B26">
-        <v>-1.115321541946846</v>
+        <v>-162121.0013304755</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2111,7 +2111,7 @@
         <v>141</v>
       </c>
       <c r="B27">
-        <v>-3.287174538105171</v>
+        <v>-35658.76390397182</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2119,7 +2119,7 @@
         <v>142</v>
       </c>
       <c r="B28">
-        <v>-5.247434727047871</v>
+        <v>-146373.757564873</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -2127,7 +2127,7 @@
         <v>143</v>
       </c>
       <c r="B29">
-        <v>-4.797316015798002</v>
+        <v>-91127.83877664992</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2135,7 +2135,7 @@
         <v>144</v>
       </c>
       <c r="B30">
-        <v>-6.256472274340981</v>
+        <v>-16008.98674444319</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2143,7 +2143,7 @@
         <v>145</v>
       </c>
       <c r="B31">
-        <v>-6.151093494875105</v>
+        <v>-217935.9639669432</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2151,7 +2151,7 @@
         <v>146</v>
       </c>
       <c r="B32">
-        <v>-44.67994728581263</v>
+        <v>-115773.6356570184</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2159,7 +2159,7 @@
         <v>147</v>
       </c>
       <c r="B33">
-        <v>1.944965591792301</v>
+        <v>-110341.1682384989</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2167,7 +2167,7 @@
         <v>148</v>
       </c>
       <c r="B34">
-        <v>-2.243779540776913</v>
+        <v>-1987.823204534051</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2175,7 +2175,7 @@
         <v>149</v>
       </c>
       <c r="B35">
-        <v>-8.265226949768403</v>
+        <v>-128609.1671047524</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2183,7 +2183,7 @@
         <v>150</v>
       </c>
       <c r="B36">
-        <v>-7.616370959188846</v>
+        <v>-241726.0097876852</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2191,7 +2191,7 @@
         <v>151</v>
       </c>
       <c r="B37">
-        <v>-1.483282879548107</v>
+        <v>-162195.6672407883</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2199,7 +2199,7 @@
         <v>152</v>
       </c>
       <c r="B38">
-        <v>-3.134810649499097</v>
+        <v>-94625.48205995531</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -2207,7 +2207,7 @@
         <v>153</v>
       </c>
       <c r="B39">
-        <v>-1.380714870602965</v>
+        <v>-203634.5519235184</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -2215,7 +2215,7 @@
         <v>154</v>
       </c>
       <c r="B40">
-        <v>-1.776311406484036</v>
+        <v>-33320.45439464282</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -2223,7 +2223,7 @@
         <v>155</v>
       </c>
       <c r="B41">
-        <v>-8.953647041230903</v>
+        <v>-83926.38109901987</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2231,7 +2231,7 @@
         <v>156</v>
       </c>
       <c r="B42">
-        <v>-9.909861547702254</v>
+        <v>-195668.984883659</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2239,7 +2239,7 @@
         <v>157</v>
       </c>
       <c r="B43">
-        <v>-4.213448715872213</v>
+        <v>-211110.1644702386</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2247,7 +2247,7 @@
         <v>158</v>
       </c>
       <c r="B44">
-        <v>-5.385505862778055</v>
+        <v>-35483.22396468927</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2255,7 +2255,7 @@
         <v>159</v>
       </c>
       <c r="B45">
-        <v>3.488955376382743</v>
+        <v>-18769.21247586677</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2263,7 +2263,7 @@
         <v>160</v>
       </c>
       <c r="B46">
-        <v>-5.560489051424652</v>
+        <v>-10235.69881707878</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2271,7 +2271,7 @@
         <v>161</v>
       </c>
       <c r="B47">
-        <v>-4.158958176791585</v>
+        <v>-12842.81292155517</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2279,7 +2279,7 @@
         <v>162</v>
       </c>
       <c r="B48">
-        <v>-7.316039593421541</v>
+        <v>-79010.38929978575</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2287,7 +2287,7 @@
         <v>163</v>
       </c>
       <c r="B49">
-        <v>-7.289875306500702</v>
+        <v>-200620.6188819679</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2295,7 +2295,7 @@
         <v>164</v>
       </c>
       <c r="B50">
-        <v>-0.7259006673047973</v>
+        <v>-42600.83313723482</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2303,7 +2303,7 @@
         <v>165</v>
       </c>
       <c r="B51">
-        <v>-0.9970936951803766</v>
+        <v>-21266.9347780156</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2311,7 +2311,7 @@
         <v>166</v>
       </c>
       <c r="B52">
-        <v>-7.341191538613029</v>
+        <v>-80451.50510525341</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2319,7 +2319,7 @@
         <v>167</v>
       </c>
       <c r="B53">
-        <v>-1.847334718331198</v>
+        <v>-62654.70544315804</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2327,7 +2327,7 @@
         <v>168</v>
       </c>
       <c r="B54">
-        <v>-4.841700222731772</v>
+        <v>-229154.7776313423</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2335,7 +2335,7 @@
         <v>169</v>
       </c>
       <c r="B55">
-        <v>-1.590478793815188</v>
+        <v>-58394.37655924061</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2343,7 +2343,7 @@
         <v>170</v>
       </c>
       <c r="B56">
-        <v>-0.853084175934047</v>
+        <v>-2148.249334986044</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2351,7 +2351,7 @@
         <v>171</v>
       </c>
       <c r="B57">
-        <v>3.476524250816077</v>
+        <v>899.6282313015802</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2359,7 +2359,7 @@
         <v>172</v>
       </c>
       <c r="B58">
-        <v>-6.179096219669634</v>
+        <v>-53638.828051637</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2367,7 +2367,7 @@
         <v>173</v>
       </c>
       <c r="B59">
-        <v>-7.28073208810277</v>
+        <v>-123773.7482993783</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2375,7 +2375,7 @@
         <v>174</v>
       </c>
       <c r="B60">
-        <v>-5.360764567991168</v>
+        <v>-107678.3263815273</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2383,7 +2383,7 @@
         <v>175</v>
       </c>
       <c r="B61">
-        <v>-29.79669932404176</v>
+        <v>-14482.90024333155</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2391,7 +2391,7 @@
         <v>176</v>
       </c>
       <c r="B62">
-        <v>-4.102240045393683</v>
+        <v>-31689.32719014174</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2399,7 +2399,7 @@
         <v>177</v>
       </c>
       <c r="B63">
-        <v>-0.7669011087998634</v>
+        <v>-105129.1832198306</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2407,7 +2407,7 @@
         <v>178</v>
       </c>
       <c r="B64">
-        <v>-7.81888080615521</v>
+        <v>-45142.22461589087</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2415,7 +2415,7 @@
         <v>179</v>
       </c>
       <c r="B65">
-        <v>-30.5627553578291</v>
+        <v>-114238.9615638382</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2423,7 +2423,7 @@
         <v>180</v>
       </c>
       <c r="B66">
-        <v>-11.71538226079978</v>
+        <v>-72092.18424853832</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2431,7 +2431,7 @@
         <v>181</v>
       </c>
       <c r="B67">
-        <v>-4.885200970407175</v>
+        <v>-336.4501636430148</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2439,7 +2439,7 @@
         <v>182</v>
       </c>
       <c r="B68">
-        <v>-0.8009642184712461</v>
+        <v>-48929.8709293689</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2447,7 +2447,7 @@
         <v>183</v>
       </c>
       <c r="B69">
-        <v>10.20367424696493</v>
+        <v>-3842.821046618011</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2455,7 +2455,7 @@
         <v>184</v>
       </c>
       <c r="B70">
-        <v>-1.891608332204107</v>
+        <v>-89892.31563692047</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2463,7 +2463,7 @@
         <v>185</v>
       </c>
       <c r="B71">
-        <v>-1.257156595101262</v>
+        <v>-10522.47375838037</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2471,7 +2471,7 @@
         <v>186</v>
       </c>
       <c r="B72">
-        <v>-21.4499176012024</v>
+        <v>-13115.98972050477</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2479,7 +2479,7 @@
         <v>187</v>
       </c>
       <c r="B73">
-        <v>-60.81521967941551</v>
+        <v>-145237.6807011696</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2487,7 +2487,7 @@
         <v>188</v>
       </c>
       <c r="B74">
-        <v>14.81329810911222</v>
+        <v>-1221.355932234729</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2495,7 +2495,7 @@
         <v>189</v>
       </c>
       <c r="B75">
-        <v>-18.14322453662115</v>
+        <v>-10152.9332431349</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2503,7 +2503,7 @@
         <v>190</v>
       </c>
       <c r="B76">
-        <v>-1.35668232984165</v>
+        <v>321.2871754682216</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2511,7 +2511,7 @@
         <v>191</v>
       </c>
       <c r="B77">
-        <v>-12.78233704975064</v>
+        <v>-51172.81636268504</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2519,7 +2519,7 @@
         <v>192</v>
       </c>
       <c r="B78">
-        <v>18.44815353485077</v>
+        <v>8583.504011654964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix arbitrage strategies algorithm;add continuous for optimal strategy
</commit_message>
<xml_diff>
--- a/data/returns_plainBS.xlsx
+++ b/data/returns_plainBS.xlsx
@@ -380,382 +380,382 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>197337.0767158029</v>
+        <v>2704.941245567406</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>297465.6189333829</v>
+        <v>6514.716256914957</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>298340.5680670611</v>
+        <v>6541.856748462156</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>212971.8628699286</v>
+        <v>-311.7903938293362</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>11529.70990781324</v>
+        <v>758.2759979959737</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>249648.2428221399</v>
+        <v>-7011.470271695271</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-64330.58858055071</v>
+        <v>-175.2173006126877</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>166988.0898869129</v>
+        <v>-1847.321007738575</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>380685.2418841907</v>
+        <v>28737.51437478181</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>40215.8651450611</v>
+        <v>-14652.46719791987</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>530153.6754074822</v>
+        <v>-41362.59818101495</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>83039.65829824925</v>
+        <v>-8566.643291131679</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>-15347.04776311174</v>
+        <v>-5698.308722559762</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>3481.558496043407</v>
+        <v>235.8624582313741</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>43637.56603912931</v>
+        <v>-1307.969830465911</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>69142.66697430113</v>
+        <v>-30706.29685933493</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>324505.4732658684</v>
+        <v>-25273.81133069033</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>237643.0335548851</v>
+        <v>-21593.5449372519</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>247965.3252162915</v>
+        <v>10182.44860650081</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>60827.70032532191</v>
+        <v>-1650.851471986621</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>501424.7261092172</v>
+        <v>-18779.76439802872</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>345566.6392755278</v>
+        <v>8429.827208441377</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>338913.7064059748</v>
+        <v>16046.81464538304</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>-1318.115157028511</v>
+        <v>-155.1987717059619</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>35366.02140131668</v>
+        <v>-11575.95744335606</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>25952.08010025875</v>
+        <v>-9868.713210854072</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>3199.398177048988</v>
+        <v>28.22197934459746</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>329190.136403135</v>
+        <v>3609.336305657495</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>259085.2281064253</v>
+        <v>11358.08695668754</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>113841.8719411928</v>
+        <v>2222.242121175183</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>509.5023271028057</v>
+        <v>25.80535520631497</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>277478.1579731206</v>
+        <v>3801.320974739631</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>165710.3123511654</v>
+        <v>14977.17682158492</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>222118.8958532696</v>
+        <v>18282.03179326902</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>44740.40358306853</v>
+        <v>4047.14896038697</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>41765.40876875295</v>
+        <v>4694.733108099043</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>2550.094631236723</v>
+        <v>349.5485817944099</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>68494.21422917293</v>
+        <v>3945.937241343303</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>260174.4170386328</v>
+        <v>33810.90244871686</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>296162.0623938176</v>
+        <v>31649.94580406183</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>-7902.601000273792</v>
+        <v>-106.1042593839938</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>63432.43220946634</v>
+        <v>9337.203172194271</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>217564.6623287912</v>
+        <v>-10892.5414086002</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>-78337.18780099883</v>
+        <v>-8308.615803979101</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>2392.791594664403</v>
+        <v>-84.1318346767689</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>56463.1891725821</v>
+        <v>-17.38217053398967</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>132288.8292391369</v>
+        <v>18720.71724375903</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>78363.28313228856</v>
+        <v>33006.71693197468</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>115262.0240638814</v>
+        <v>12316.39870072939</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>108230.1907798635</v>
+        <v>7420.199415782768</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>191548.8038520592</v>
+        <v>13125.88972320877</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>57992.40052240118</v>
+        <v>5354.799747064203</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>41898.52605399358</v>
+        <v>1818.950526082811</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>55128.61046578563</v>
+        <v>2421.867774025884</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>42649.85457789512</v>
+        <v>117.1642113311409</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>-5002.819444262171</v>
+        <v>153.8637061300788</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58">
-        <v>-435.7708803751999</v>
+        <v>-12.51980375771075</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59">
-        <v>163623.4701065382</v>
+        <v>21974.0373464909</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <v>141413.7680202851</v>
+        <v>13845.17008296532</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61">
-        <v>208577.9650663869</v>
+        <v>30795.60528427632</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62">
-        <v>27843.31088296386</v>
+        <v>7625.454311797399</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63">
-        <v>-111655.5227430478</v>
+        <v>-6748.196841921219</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>131482.6375780694</v>
+        <v>7928.093995865041</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65">
-        <v>67466.82605130819</v>
+        <v>5359.202943843336</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66">
-        <v>-53.15769916871658</v>
+        <v>-5549.440000077097</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67">
-        <v>2294.315538587604</v>
+        <v>121.7331531027298</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <v>115719.0837642277</v>
+        <v>20931.09962877977</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69">
-        <v>101250.0179765426</v>
+        <v>36618.20906090448</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>39557.60128527856</v>
+        <v>2818.423501531342</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71">
-        <v>296497.7650966039</v>
+        <v>1624.880194766267</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72">
-        <v>1779.995740417664</v>
+        <v>128.220072864367</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <v>-830.1630348725596</v>
+        <v>-186.8994348410242</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <v>44616.09122968344</v>
+        <v>8070.531630054465</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <v>44639.51131772243</v>
+        <v>1468.278598325155</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76">
-        <v>38371.09653527031</v>
+        <v>7465.711755332242</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77">
-        <v>28366.9552980102</v>
+        <v>6238.969377969336</v>
       </c>
     </row>
   </sheetData>
@@ -778,282 +778,282 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>-92044.44378991987</v>
+        <v>3682.306956020851</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>-258032.965518698</v>
+        <v>-2828.385535374186</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>5902.233069072514</v>
+        <v>5647.787362296564</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>397030.8338200637</v>
+        <v>16067.51779907378</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>-323291.1634107444</v>
+        <v>10000.92827659918</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>-82858.78866921402</v>
+        <v>18462.85896625027</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-292783.5177418821</v>
+        <v>-2406.917105007136</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>18337.55189908201</v>
+        <v>745.6130109155279</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <v>22742.67502138755</v>
+        <v>12260.12891497729</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <v>-37938.49502184596</v>
+        <v>5483.100395180862</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <v>-426970.7512380974</v>
+        <v>21751.38143100297</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <v>10808.55671523164</v>
+        <v>666.5933600446788</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <v>-155196.2402139521</v>
+        <v>14174.85050381131</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <v>-117641.8170871335</v>
+        <v>87826.13860023701</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16">
-        <v>-49232.43882227142</v>
+        <v>10194.98513464503</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>-89508.95583615307</v>
+        <v>21857.9205077245</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>-216402.8759142413</v>
+        <v>26269.37824007923</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <v>-106717.3662770389</v>
+        <v>-5570.752878463286</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20">
-        <v>-25275.91078970179</v>
+        <v>9291.106452880911</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21">
-        <v>-234377.0366289244</v>
+        <v>7585.015158869613</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <v>-121821.8121935435</v>
+        <v>87856.11643422626</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <v>-89945.69326719249</v>
+        <v>-11073.75159840068</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24">
-        <v>-217785.1339405923</v>
+        <v>177498.8408329274</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25">
-        <v>-76.67387321348518</v>
+        <v>-1.838546900772371</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <v>-72120.61865482164</v>
+        <v>-2174.240596121712</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <v>-187327.2303255536</v>
+        <v>-11809.77940596812</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28">
-        <v>-169565.5004059972</v>
+        <v>-23011.18117743199</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29">
-        <v>-40446.75910225509</v>
+        <v>-8.83330089682886</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30">
-        <v>-20876.28168956712</v>
+        <v>-3190.916301602745</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>214.7078604051971</v>
+        <v>11.9459057438188</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32">
-        <v>-95753.43575020511</v>
+        <v>-6307.216499937009</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33">
-        <v>-127933.4220018526</v>
+        <v>-760.3066751415854</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>-55834.43636002701</v>
+        <v>33378.51874128314</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35">
-        <v>-119812.1497073229</v>
+        <v>-9521.94113906977</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36">
-        <v>-59524.13283159105</v>
+        <v>-15563.15288752221</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37">
-        <v>-195562.0171427578</v>
+        <v>-29479.19280221562</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38">
-        <v>-55309.98671481234</v>
+        <v>-21811.61542938649</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
-        <v>-2256.570539664935</v>
+        <v>19149.39087216876</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40">
-        <v>-64048.62597859876</v>
+        <v>-4567.815319089983</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41">
-        <v>-96440.02990230816</v>
+        <v>-6348.439430727806</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42">
-        <v>-86246.11162811198</v>
+        <v>429.6237318063013</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43">
-        <v>-37651.44016981644</v>
+        <v>-4659.890386788288</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44">
-        <v>-113326.0860243698</v>
+        <v>44958.97128226097</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45">
-        <v>-40410.09925275421</v>
+        <v>24344.87496869027</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46">
-        <v>-106736.9307067019</v>
+        <v>2738.67999197395</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47">
-        <v>-71812.63322241521</v>
+        <v>230.8849723767835</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48">
-        <v>-293.2486704946933</v>
+        <v>5728.448025208311</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49">
-        <v>-14004.36792985534</v>
+        <v>-1628.139431820802</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50">
-        <v>-8992.117755777894</v>
+        <v>-1495.616651977709</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51">
-        <v>-58562.53493303689</v>
+        <v>-19434.48058535961</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52">
-        <v>-10081.10175316761</v>
+        <v>-4246.370963431777</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53">
-        <v>-141176.264849343</v>
+        <v>3350.897745242667</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54">
-        <v>-1245.073653759623</v>
+        <v>-7.200611128759647</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55">
-        <v>-12900.84184462313</v>
+        <v>-35.61232654289279</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56">
-        <v>-69928.64412166183</v>
+        <v>-1342.121738051051</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57">
-        <v>8241.597735539988</v>
+        <v>155.9095762360048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>